<commit_message>
Make AI Great Again
</commit_message>
<xml_diff>
--- a/programming/ohands/model_analysis_results.xlsx
+++ b/programming/ohands/model_analysis_results.xlsx
@@ -20,13 +20,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +48,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -416,14 +428,92 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>distilgpt2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>gpt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>parameters</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>81912576</v>
+      </c>
+      <c r="C2" t="n">
+        <v>124439808</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>layers</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>86</v>
+      </c>
+      <c r="C3" t="n">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>vocab_size</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>50257</v>
+      </c>
+      <c r="C4" t="n">
+        <v>50257</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>hidden_size</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>768</v>
+      </c>
+      <c r="C5" t="n">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>num_attention_heads</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>12</v>
+      </c>
+      <c r="C6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -434,14 +524,66 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>distilgpt2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>gpt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>avg_inference_time</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>5.574</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9.651</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>tokens_per_second</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8.970000000000001</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5.181</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>std_inference_time</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.038</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -452,14 +594,66 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>distilgpt2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>gpt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>lexical_diversity</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.235</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>avg_length</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>43.667</v>
+      </c>
+      <c r="C3" t="n">
+        <v>64.667</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>repetition_rate</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.654</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -470,14 +664,53 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>distilgpt2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>gpt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>model_size_mb</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>156.24</v>
+      </c>
+      <c r="C2" t="n">
+        <v>237.35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>vocab_size_mb</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>